<commit_message>
new GenerateLanguage Action, json
</commit_message>
<xml_diff>
--- a/Code/9-Extensions/ItemTemplates/GenerateLanguagesExcel/Strings.xlsx
+++ b/Code/9-Extensions/ItemTemplates/GenerateLanguagesExcel/Strings.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Lever\Code\9-Extensions\ItemTemplates\LanguagesExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Lever\Code\9-Extensions\ItemTemplates\GenerateLanguagesExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9195C20B-3A1F-46D7-8AC9-93575D24E855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="7065" yWindow="2475" windowWidth="18645" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Languages" sheetId="1" r:id="rId1"/>
-    <sheet name="References" sheetId="2" r:id="rId2"/>
+    <sheet name="__Config" sheetId="3" r:id="rId1"/>
+    <sheet name="Languages" sheetId="1" r:id="rId2"/>
+    <sheet name="References" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="544">
   <si>
     <t>Identifier</t>
   </si>
@@ -1650,18 +1652,25 @@
     <t>EnglishName</t>
   </si>
   <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>GenerateStrings</t>
+  </si>
+  <si>
     <t>NativeName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1670,19 +1679,26 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1692,6 +1708,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1708,7 +1730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1718,6 +1740,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2037,7 +2062,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166B4647-FED3-47DE-B585-45CA823CB992}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{5FF194A7-56E9-482B-A40C-A21856B0FE15}">
+      <formula1>"GenerateStrings,GenerateJsons"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2047,12 +2107,12 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="26.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="36.28515625" customWidth="1"/>
+    <col min="1" max="5" width="36.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2069,7 +2129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2093,25 +2153,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="6.875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="9.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="36.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.875" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>537</v>
       </c>
@@ -2125,10 +2185,10 @@
         <v>540</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>127</v>
       </c>
@@ -2142,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>54</v>
       </c>
@@ -2159,7 +2219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>94</v>
       </c>
@@ -2176,7 +2236,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -2193,7 +2253,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>122</v>
       </c>
@@ -2210,7 +2270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>77</v>
       </c>
@@ -2227,7 +2287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>44</v>
       </c>
@@ -2244,7 +2304,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>29740</v>
       </c>
@@ -2261,7 +2321,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>30764</v>
       </c>
@@ -2278,7 +2338,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>109</v>
       </c>
@@ -2295,7 +2355,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>35</v>
       </c>
@@ -2312,7 +2372,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>2</v>
       </c>
@@ -2329,7 +2389,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>69</v>
       </c>
@@ -2346,7 +2406,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>81</v>
       </c>
@@ -2363,7 +2423,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>126</v>
       </c>
@@ -2380,7 +2440,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>30746</v>
       </c>
@@ -2397,7 +2457,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>25626</v>
       </c>
@@ -2414,7 +2474,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>26650</v>
       </c>
@@ -2431,7 +2491,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>3</v>
       </c>
@@ -2448,7 +2508,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>131</v>
       </c>
@@ -2465,7 +2525,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>5</v>
       </c>
@@ -2482,7 +2542,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>82</v>
       </c>
@@ -2499,7 +2559,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>6</v>
       </c>
@@ -2516,7 +2576,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>7</v>
       </c>
@@ -2533,7 +2593,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>31790</v>
       </c>
@@ -2550,7 +2610,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>101</v>
       </c>
@@ -2567,7 +2627,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>8</v>
       </c>
@@ -2584,7 +2644,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>9</v>
       </c>
@@ -2601,7 +2661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>10</v>
       </c>
@@ -2618,7 +2678,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>37</v>
       </c>
@@ -2635,7 +2695,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>45</v>
       </c>
@@ -2652,7 +2712,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>41</v>
       </c>
@@ -2669,7 +2729,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>11</v>
       </c>
@@ -2686,7 +2746,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>100</v>
       </c>
@@ -2703,7 +2763,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>56</v>
       </c>
@@ -2720,7 +2780,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>12</v>
       </c>
@@ -2737,7 +2797,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>98</v>
       </c>
@@ -2754,7 +2814,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>60</v>
       </c>
@@ -2771,7 +2831,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>145</v>
       </c>
@@ -2788,7 +2848,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>86</v>
       </c>
@@ -2805,7 +2865,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>132</v>
       </c>
@@ -2822,7 +2882,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>71</v>
       </c>
@@ -2839,7 +2899,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>104</v>
       </c>
@@ -2856,7 +2916,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>31848</v>
       </c>
@@ -2873,7 +2933,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>13</v>
       </c>
@@ -2890,7 +2950,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>57</v>
       </c>
@@ -2907,7 +2967,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>26</v>
       </c>
@@ -2924,7 +2984,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>46</v>
       </c>
@@ -2941,7 +3001,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>14</v>
       </c>
@@ -2958,7 +3018,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>43</v>
       </c>
@@ -2975,7 +3035,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>33</v>
       </c>
@@ -2992,7 +3052,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>112</v>
       </c>
@@ -3009,7 +3069,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>120</v>
       </c>
@@ -3026,7 +3086,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>15</v>
       </c>
@@ -3043,7 +3103,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>16</v>
       </c>
@@ -3060,7 +3120,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>93</v>
       </c>
@@ -3077,7 +3137,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>30813</v>
       </c>
@@ -3094,7 +3154,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>31837</v>
       </c>
@@ -3111,7 +3171,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>17</v>
       </c>
@@ -3128,7 +3188,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>55</v>
       </c>
@@ -3145,7 +3205,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>63</v>
       </c>
@@ -3162,7 +3222,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>111</v>
       </c>
@@ -3179,7 +3239,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>83</v>
       </c>
@@ -3196,7 +3256,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>75</v>
       </c>
@@ -3213,7 +3273,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>18</v>
       </c>
@@ -3230,7 +3290,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>87</v>
       </c>
@@ -3247,7 +3307,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>64</v>
       </c>
@@ -3264,7 +3324,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>110</v>
       </c>
@@ -3281,7 +3341,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>84</v>
       </c>
@@ -3298,7 +3358,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>39</v>
       </c>
@@ -3315,7 +3375,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>38</v>
       </c>
@@ -3332,7 +3392,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>129</v>
       </c>
@@ -3349,7 +3409,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>47</v>
       </c>
@@ -3366,7 +3426,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>76</v>
       </c>
@@ -3383,7 +3443,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>80</v>
       </c>
@@ -3400,7 +3460,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>30800</v>
       </c>
@@ -3417,7 +3477,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>31824</v>
       </c>
@@ -3434,7 +3494,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>124</v>
       </c>
@@ -3451,7 +3511,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>78</v>
       </c>
@@ -3468,7 +3528,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>62</v>
       </c>
@@ -3485,7 +3545,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>58</v>
       </c>
@@ -3502,7 +3562,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>31764</v>
       </c>
@@ -3519,7 +3579,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>97</v>
       </c>
@@ -3536,7 +3596,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>19</v>
       </c>
@@ -3553,7 +3613,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>30740</v>
       </c>
@@ -3570,7 +3630,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>20</v>
       </c>
@@ -3587,7 +3647,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>108</v>
       </c>
@@ -3604,7 +3664,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>130</v>
       </c>
@@ -3621,7 +3681,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>72</v>
       </c>
@@ -3638,7 +3698,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>70</v>
       </c>
@@ -3655,7 +3715,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>21</v>
       </c>
@@ -3672,7 +3732,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>140</v>
       </c>
@@ -3689,7 +3749,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>99</v>
       </c>
@@ -3706,7 +3766,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>22</v>
       </c>
@@ -3723,7 +3783,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>134</v>
       </c>
@@ -3740,7 +3800,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>107</v>
       </c>
@@ -3757,7 +3817,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>23</v>
       </c>
@@ -3774,7 +3834,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>24</v>
       </c>
@@ -3791,7 +3851,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>25</v>
       </c>
@@ -3808,7 +3868,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>135</v>
       </c>
@@ -3825,7 +3885,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>79</v>
       </c>
@@ -3842,7 +3902,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>133</v>
       </c>
@@ -3859,7 +3919,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>59</v>
       </c>
@@ -3876,7 +3936,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>91</v>
       </c>
@@ -3893,7 +3953,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>27</v>
       </c>
@@ -3910,7 +3970,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>36</v>
       </c>
@@ -3927,7 +3987,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>30779</v>
       </c>
@@ -3944,7 +4004,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>31803</v>
       </c>
@@ -3961,7 +4021,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>28731</v>
       </c>
@@ -3978,7 +4038,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>29755</v>
       </c>
@@ -3995,7 +4055,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>28</v>
       </c>
@@ -4012,7 +4072,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>31770</v>
       </c>
@@ -4029,7 +4089,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>27674</v>
       </c>
@@ -4046,7 +4106,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>28698</v>
       </c>
@@ -4063,7 +4123,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>29</v>
       </c>
@@ -4080,7 +4140,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>65</v>
       </c>
@@ -4097,7 +4157,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>90</v>
       </c>
@@ -4114,7 +4174,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>73</v>
       </c>
@@ -4131,7 +4191,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>74</v>
       </c>
@@ -4148,7 +4208,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>40</v>
       </c>
@@ -4165,7 +4225,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>31784</v>
       </c>
@@ -4182,7 +4242,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>30</v>
       </c>
@@ -4199,7 +4259,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>66</v>
       </c>
@@ -4216,7 +4276,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>50</v>
       </c>
@@ -4233,7 +4293,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>31</v>
       </c>
@@ -4250,7 +4310,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>68</v>
       </c>
@@ -4267,7 +4327,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>95</v>
       </c>
@@ -4284,7 +4344,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>31839</v>
       </c>
@@ -4301,7 +4361,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>128</v>
       </c>
@@ -4318,7 +4378,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>34</v>
       </c>
@@ -4335,7 +4395,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>32</v>
       </c>
@@ -4352,7 +4412,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>67</v>
       </c>
@@ -4369,7 +4429,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>30787</v>
       </c>
@@ -4386,7 +4446,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>31811</v>
       </c>
@@ -4403,7 +4463,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>42</v>
       </c>
@@ -4420,7 +4480,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -4437,7 +4497,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>52</v>
       </c>
@@ -4454,7 +4514,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>106</v>
       </c>
@@ -4471,7 +4531,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>30724</v>
       </c>
@@ -4488,7 +4548,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>4</v>
       </c>
@@ -4505,7 +4565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>31748</v>
       </c>
@@ -4522,7 +4582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>53</v>
       </c>
@@ -4540,6 +4600,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>